<commit_message>
Updated SPI's on CON1 and CON2
Updated SPI's on CON1 and CON2.
</commit_message>
<xml_diff>
--- a/Accessories/Encoder Board/Project Outputs for Encoder_Expansion_Board_Project/BOM_Encoder_Expansion_Board_Project.xlsx
+++ b/Accessories/Encoder Board/Project Outputs for Encoder_Expansion_Board_Project/BOM_Encoder_Expansion_Board_Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Altium\Encoder Board\Project Outputs for Encoder_Expansion_Board_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594461D4-ADDD-4B72-82A1-581DBB7D97A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849242AF-30B3-41FE-B4E5-A35155475224}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,15 +102,6 @@
     <t>PEC12R-4220F-S0024</t>
   </si>
   <si>
-    <t>Jumper2</t>
-  </si>
-  <si>
-    <t>JP1, JP2</t>
-  </si>
-  <si>
-    <t>PIN_HEADER_1x2</t>
-  </si>
-  <si>
     <t>Resistor</t>
   </si>
   <si>
@@ -163,16 +154,48 @@
   </si>
   <si>
     <t>Resistor 10K</t>
+  </si>
+  <si>
+    <t>Jumper3</t>
+  </si>
+  <si>
+    <t>PIN_HEADER_1x3</t>
+  </si>
+  <si>
+    <t>JP1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -280,16 +303,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,45 +633,47 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="20.140625" customWidth="1"/>
     <col min="7" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.140625" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>38</v>
+      <c r="G1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -660,18 +688,18 @@
       <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>4</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>0.4</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -686,18 +714,18 @@
       <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="4">
         <v>1</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="4">
         <v>3.27</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="4">
         <v>29.68</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -712,18 +740,18 @@
       <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <v>1</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="4">
         <v>0.81</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <v>6.87</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -738,170 +766,170 @@
       <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="4">
         <v>1</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="4">
         <v>1.59</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <v>14.03</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>25</v>
+      <c r="A6" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="4">
+        <v>5</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="4">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="D9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="4">
         <v>2</v>
       </c>
-      <c r="G6" s="6">
-        <v>0.26</v>
-      </c>
-      <c r="H6" s="6">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="G9" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="4">
         <v>1</v>
       </c>
-      <c r="G7" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="H7" s="6">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="6">
-        <v>5</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="H8" s="6">
-        <v>2.65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="6">
-        <v>2</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="H9" s="6">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="6">
-        <v>1</v>
-      </c>
-      <c r="G10" s="6">
+      <c r="G10" s="4">
         <v>1.64</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="4">
         <v>14.63</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G11">
         <f>SUM(G2:G10)</f>
-        <v>8.77</v>
+        <v>8.64</v>
       </c>
       <c r="H11">
         <f>SUM(H2:H10)</f>
-        <v>72.61</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>39</v>
+        <v>71.709999999999994</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G12">
         <f>SUM(G2:G10)</f>
-        <v>8.77</v>
+        <v>8.64</v>
       </c>
       <c r="H12">
         <f>SUM(H2:H10)/10</f>
-        <v>7.2610000000000001</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>40</v>
+        <v>7.1709999999999994</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>